<commit_message>
Major updates including first Rmarkdown chunk
</commit_message>
<xml_diff>
--- a/pcaoutput.xlsx
+++ b/pcaoutput.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="17">
   <si>
     <t>var</t>
   </si>
@@ -45,6 +45,24 @@
   </si>
   <si>
     <t>OD_cm</t>
+  </si>
+  <si>
+    <t>Respiration</t>
+  </si>
+  <si>
+    <t>BG</t>
+  </si>
+  <si>
+    <t>NAG</t>
+  </si>
+  <si>
+    <t>Phosphatase</t>
+  </si>
+  <si>
+    <t>Chlorophyll</t>
+  </si>
+  <si>
+    <t>Biomass</t>
   </si>
 </sst>
 </file>
@@ -106,7 +124,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="132">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="1"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2"/>
@@ -198,6 +216,87 @@
       <alignment wrapText="true"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
@@ -431,101 +530,101 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="78">
+      <c r="A1" t="s" s="105">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="79">
+      <c r="B1" t="s" s="106">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="80">
+      <c r="C1" t="s" s="107">
         <v>2</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="81">
-        <v>3</v>
-      </c>
-      <c r="B2" t="n" s="89">
+      <c r="A2" t="s" s="108">
+        <v>11</v>
+      </c>
+      <c r="B2" t="n" s="116">
         <v>-0.26814948418346574</v>
       </c>
-      <c r="C2" t="n" s="97">
+      <c r="C2" t="n" s="124">
         <v>0.5192179509324171</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="82">
+      <c r="A3" t="s" s="109">
         <v>4</v>
       </c>
-      <c r="B3" t="n" s="90">
+      <c r="B3" t="n" s="117">
         <v>0.26953776773085636</v>
       </c>
-      <c r="C3" t="n" s="98">
+      <c r="C3" t="n" s="125">
         <v>0.35550112865942224</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="83">
+      <c r="A4" t="s" s="110">
         <v>5</v>
       </c>
-      <c r="B4" t="n" s="91">
+      <c r="B4" t="n" s="118">
         <v>-0.02493302687316057</v>
       </c>
-      <c r="C4" t="n" s="99">
+      <c r="C4" t="n" s="126">
         <v>0.7398258595361964</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s" s="84">
-        <v>6</v>
-      </c>
-      <c r="B5" t="n" s="92">
+      <c r="A5" t="s" s="111">
+        <v>12</v>
+      </c>
+      <c r="B5" t="n" s="119">
         <v>0.5066925002902241</v>
       </c>
-      <c r="C5" t="n" s="100">
+      <c r="C5" t="n" s="127">
         <v>3.2712037364376195E-4</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s" s="85">
-        <v>7</v>
-      </c>
-      <c r="B6" t="n" s="93">
+      <c r="A6" t="s" s="112">
+        <v>13</v>
+      </c>
+      <c r="B6" t="n" s="120">
         <v>0.47782810970682676</v>
       </c>
-      <c r="C6" t="n" s="101">
+      <c r="C6" t="n" s="128">
         <v>-0.03387065164638178</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s" s="86">
-        <v>8</v>
-      </c>
-      <c r="B7" t="n" s="94">
+      <c r="A7" t="s" s="113">
+        <v>14</v>
+      </c>
+      <c r="B7" t="n" s="121">
         <v>0.45529800415595756</v>
       </c>
-      <c r="C7" t="n" s="102">
+      <c r="C7" t="n" s="129">
         <v>0.05105067453415059</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s" s="87">
-        <v>9</v>
-      </c>
-      <c r="B8" t="n" s="95">
+      <c r="A8" t="s" s="114">
+        <v>15</v>
+      </c>
+      <c r="B8" t="n" s="122">
         <v>0.1957827684785475</v>
       </c>
-      <c r="C8" t="n" s="103">
+      <c r="C8" t="n" s="130">
         <v>-0.0966894417767627</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s" s="88">
-        <v>10</v>
-      </c>
-      <c r="B9" t="n" s="96">
+      <c r="A9" t="s" s="115">
+        <v>16</v>
+      </c>
+      <c r="B9" t="n" s="123">
         <v>0.35233426284122454</v>
       </c>
-      <c r="C9" t="n" s="104">
+      <c r="C9" t="n" s="131">
         <v>0.20877503907499212</v>
       </c>
     </row>

</xml_diff>